<commit_message>
dgkanatsios 1.22 fork WIP
</commit_message>
<xml_diff>
--- a/CKAD/notes/1.22-curiculum.xlsx
+++ b/CKAD/notes/1.22-curiculum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Projects\KubeWorks\CKAD\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422873D1-F3F2-4AC3-B877-AECB3A8B834C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52DD152-6491-44CE-9496-411636241991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{394FC45E-8109-49DF-99A9-124735A88F84}"/>
   </bookViews>
@@ -34,19 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
-  <si>
-    <t>Application  Design  and  Build</t>
-  </si>
-  <si>
-    <t>Application  Deployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Application  Environment, Configuration  and  Security</t>
-  </si>
-  <si>
-    <t>Application  observability  and maintenance</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Services &amp; Networking</t>
   </si>
@@ -115,6 +103,39 @@
   </si>
   <si>
     <t> Use Ingress rules to expose applications</t>
+  </si>
+  <si>
+    <t>Application  Design  and  Build 20%</t>
+  </si>
+  <si>
+    <t>Application  Deployment 20 %</t>
+  </si>
+  <si>
+    <t>Application  observability  and maintenance 15%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Application  Environment, Configuration  and  Security 25%</t>
+  </si>
+  <si>
+    <t>Services &amp; Networking 20%</t>
+  </si>
+  <si>
+    <t>Multi-Container Pods</t>
+  </si>
+  <si>
+    <t>Pod Design</t>
+  </si>
+  <si>
+    <t>State Persistence</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Observability</t>
+  </si>
+  <si>
+    <t>Configuration</t>
   </si>
 </sst>
 </file>
@@ -152,7 +173,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,184 +490,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD0DBBD-D29C-4CD7-8788-993495A2A223}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" customWidth="1"/>
+    <col min="1" max="1" width="56.5703125" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>26</v>
+      <c r="C26" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>